<commit_message>
Update to read CSV files and adjust question page
</commit_message>
<xml_diff>
--- a/data/skills_diagnosis_questions.xlsx
+++ b/data/skills_diagnosis_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_tekishokusindanwebsite\website\myapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C915D4B-9FE5-4359-9048-17C60937AF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC7E001-0B94-4575-88F9-00F22D4E5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E976E6D5-9A0B-4A74-A535-633DBA01C206}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
   <si>
     <t>軸名１</t>
     <rPh sb="0" eb="2">
@@ -74,26 +74,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>得意なこと1（論理）</t>
-    <rPh sb="0" eb="2">
-      <t>トクイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ロンリ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>得意なこと2（感情）</t>
-    <rPh sb="0" eb="2">
-      <t>トクイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>カンジョウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>仕事上の課題に直面したとき、どのように対処しますか？</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -232,23 +212,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>得意なこと3(精密性)</t>
-    <rPh sb="0" eb="2">
-      <t>トクイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>セイミツ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>セイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>得意なこと4(全体像)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>プロジェクトを進める際、どのように取り組みますか？</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -381,14 +344,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>得意なこと5(伝統性)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>得意なこと6(創造性)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>仕事の進め方を考えるとき、どちらの方法を選択しますか？</t>
     <rPh sb="7" eb="8">
       <t>カンガ</t>
@@ -495,14 +450,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>7得意なこと(熟考)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>得意なこと8(即座)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>重要な決断をする際、どのように行動しますか？</t>
   </si>
   <si>
@@ -616,14 +563,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>得意なこと9(身体能力)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>得意なこと10(学力)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>どのような作業が得意ですか？</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -743,6 +682,80 @@
     <rPh sb="0" eb="2">
       <t>ベンキョウ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>論理</t>
+    <rPh sb="0" eb="2">
+      <t>ロンリ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>感情</t>
+    <rPh sb="0" eb="2">
+      <t>カンジョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>精密性</t>
+    <rPh sb="0" eb="3">
+      <t>セイミツセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>全体像</t>
+    <rPh sb="0" eb="3">
+      <t>ゼンタイゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>伝統性</t>
+    <rPh sb="0" eb="3">
+      <t>デントウセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>創造性</t>
+    <rPh sb="0" eb="3">
+      <t>ソウゾウセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>熟考</t>
+    <rPh sb="0" eb="2">
+      <t>ジュッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>即座</t>
+    <rPh sb="0" eb="2">
+      <t>ソクザ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>身体能力</t>
+    <rPh sb="0" eb="4">
+      <t>シンタイノウリョク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>学力</t>
+    <rPh sb="0" eb="2">
+      <t>ガクリョク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1143,464 +1156,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7185FFB-A2DC-4304-AE7D-CB32CF5E3F89}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5" customWidth="1"/>
-    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="B26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>